<commit_message>
Round volume calculation to one decimal place
</commit_message>
<xml_diff>
--- a/CleanData/Excel/nitrogenData.xlsx
+++ b/CleanData/Excel/nitrogenData.xlsx
@@ -492,7 +492,7 @@
         <v>15.1</v>
       </c>
       <c r="O2">
-        <v>1623.646292808686</v>
+        <v>1623.6</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +553,7 @@
         <v>13.7</v>
       </c>
       <c r="O3">
-        <v>1228.428177400559</v>
+        <v>1228.4</v>
       </c>
     </row>
     <row r="4">
@@ -614,7 +614,7 @@
         <v>14.9</v>
       </c>
       <c r="O4">
-        <v>1615.793881971039</v>
+        <v>1615.8</v>
       </c>
     </row>
     <row r="5">
@@ -675,7 +675,7 @@
         <v>13.5</v>
       </c>
       <c r="O5">
-        <v>1192.823460659874</v>
+        <v>1192.8</v>
       </c>
     </row>
     <row r="6">
@@ -736,7 +736,7 @@
         <v>11.7</v>
       </c>
       <c r="O6">
-        <v>723.9219075556763</v>
+        <v>723.9</v>
       </c>
     </row>
     <row r="7">
@@ -797,7 +797,7 @@
         <v>14.6</v>
       </c>
       <c r="O7">
-        <v>1372.806874580361</v>
+        <v>1372.8</v>
       </c>
     </row>
     <row r="8">
@@ -858,7 +858,7 @@
         <v>12.7</v>
       </c>
       <c r="O8">
-        <v>1055.64058145312</v>
+        <v>1055.6</v>
       </c>
     </row>
     <row r="9">
@@ -919,7 +919,7 @@
         <v>12.3</v>
       </c>
       <c r="O9">
-        <v>950.5831051231996</v>
+        <v>950.6</v>
       </c>
     </row>
     <row r="10">
@@ -980,7 +980,7 @@
         <v>14.6</v>
       </c>
       <c r="O10">
-        <v>1529.061315589507</v>
+        <v>1529.1</v>
       </c>
     </row>
     <row r="11">
@@ -1041,7 +1041,7 @@
         <v>13.3</v>
       </c>
       <c r="O11">
-        <v>1204.05203640258</v>
+        <v>1204.1</v>
       </c>
     </row>
     <row r="12">
@@ -1102,7 +1102,7 @@
         <v>12.7</v>
       </c>
       <c r="O12">
-        <v>1030.305207498245</v>
+        <v>1030.3</v>
       </c>
     </row>
     <row r="13">
@@ -1163,7 +1163,7 @@
         <v>13.4</v>
       </c>
       <c r="O13">
-        <v>1156.413972601096</v>
+        <v>1156.4</v>
       </c>
     </row>
     <row r="14">
@@ -1224,7 +1224,7 @@
         <v>15.2</v>
       </c>
       <c r="O14">
-        <v>1500.056037816464</v>
+        <v>1500.1</v>
       </c>
     </row>
     <row r="15">
@@ -1285,7 +1285,7 @@
         <v>14.4</v>
       </c>
       <c r="O15">
-        <v>1411.454747404822</v>
+        <v>1411.5</v>
       </c>
     </row>
     <row r="16">
@@ -1346,7 +1346,7 @@
         <v>12.6</v>
       </c>
       <c r="O16">
-        <v>1055.707078497621</v>
+        <v>1055.7</v>
       </c>
     </row>
     <row r="17">
@@ -1407,7 +1407,7 @@
         <v>13.7</v>
       </c>
       <c r="O17">
-        <v>1179.291050304536</v>
+        <v>1179.3</v>
       </c>
     </row>
     <row r="18">
@@ -1468,7 +1468,7 @@
         <v>13.8</v>
       </c>
       <c r="O18">
-        <v>1276.341130559233</v>
+        <v>1276.3</v>
       </c>
     </row>
     <row r="19">
@@ -1529,7 +1529,7 @@
         <v>13.1</v>
       </c>
       <c r="O19">
-        <v>1006.373601860749</v>
+        <v>1006.4</v>
       </c>
     </row>
     <row r="20">
@@ -1590,7 +1590,7 @@
         <v>13.7</v>
       </c>
       <c r="O20">
-        <v>1238.255602819763</v>
+        <v>1238.3</v>
       </c>
     </row>
     <row r="21">
@@ -1651,7 +1651,7 @@
         <v>14</v>
       </c>
       <c r="O21">
-        <v>1293.079536217559</v>
+        <v>1293.1</v>
       </c>
     </row>
     <row r="22">
@@ -1712,7 +1712,7 @@
         <v>13.3</v>
       </c>
       <c r="O22">
-        <v>1129.956526470114</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="23">
@@ -1773,7 +1773,7 @@
         <v>13</v>
       </c>
       <c r="O23">
-        <v>955.672485222015</v>
+        <v>955.7000000000001</v>
       </c>
     </row>
     <row r="24">
@@ -1834,7 +1834,7 @@
         <v>13.1</v>
       </c>
       <c r="O24">
-        <v>970.4316875085799</v>
+        <v>970.4</v>
       </c>
     </row>
     <row r="25">
@@ -1895,7 +1895,7 @@
         <v>13.7</v>
       </c>
       <c r="O25">
-        <v>1385.66698410783</v>
+        <v>1385.7</v>
       </c>
     </row>
     <row r="26">
@@ -1956,7 +1956,7 @@
         <v>13.1</v>
       </c>
       <c r="O26">
-        <v>1141.155780681386</v>
+        <v>1141.2</v>
       </c>
     </row>
     <row r="27">
@@ -2017,7 +2017,7 @@
         <v>13.5</v>
       </c>
       <c r="O27">
-        <v>1068.769820751247</v>
+        <v>1068.8</v>
       </c>
     </row>
     <row r="28">
@@ -2078,7 +2078,7 @@
         <v>14.7</v>
       </c>
       <c r="O28">
-        <v>1436.934634621762</v>
+        <v>1436.9</v>
       </c>
     </row>
     <row r="29">
@@ -2139,7 +2139,7 @@
         <v>14.6</v>
       </c>
       <c r="O29">
-        <v>1495.578221087547</v>
+        <v>1495.6</v>
       </c>
     </row>
     <row r="30">
@@ -2200,7 +2200,7 @@
         <v>13.6</v>
       </c>
       <c r="O30">
-        <v>1258.982783950597</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="31">
@@ -2261,7 +2261,7 @@
         <v>15.4</v>
       </c>
       <c r="O31">
-        <v>1663.96758731996</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="32">
@@ -2322,7 +2322,7 @@
         <v>13.2</v>
       </c>
       <c r="O32">
-        <v>1103.905392988996</v>
+        <v>1103.9</v>
       </c>
     </row>
     <row r="33">
@@ -2383,7 +2383,7 @@
         <v>12.1</v>
       </c>
       <c r="O33">
-        <v>958.2512091918366</v>
+        <v>958.3</v>
       </c>
     </row>
     <row r="34">
@@ -2444,7 +2444,7 @@
         <v>12.5</v>
       </c>
       <c r="O34">
-        <v>850.8480103472357</v>
+        <v>850.8</v>
       </c>
     </row>
     <row r="35">
@@ -2505,7 +2505,7 @@
         <v>15.2</v>
       </c>
       <c r="O35">
-        <v>1536.347716150733</v>
+        <v>1536.3</v>
       </c>
     </row>
     <row r="36">
@@ -2566,7 +2566,7 @@
         <v>13.4</v>
       </c>
       <c r="O36">
-        <v>1165.815712215739</v>
+        <v>1165.8</v>
       </c>
     </row>
     <row r="37">
@@ -2627,7 +2627,7 @@
         <v>13.8</v>
       </c>
       <c r="O37">
-        <v>1226.484055146763</v>
+        <v>1226.5</v>
       </c>
     </row>
     <row r="38">
@@ -2688,7 +2688,7 @@
         <v>12.7</v>
       </c>
       <c r="O38">
-        <v>996.5247088917455</v>
+        <v>996.5</v>
       </c>
     </row>
     <row r="39">
@@ -2749,7 +2749,7 @@
         <v>14.3</v>
       </c>
       <c r="O39">
-        <v>1370.505134362831</v>
+        <v>1370.5</v>
       </c>
     </row>
     <row r="40">
@@ -2810,7 +2810,7 @@
         <v>14.1</v>
       </c>
       <c r="O40">
-        <v>1269.979405435713</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="41">
@@ -2871,7 +2871,7 @@
         <v>13.2</v>
       </c>
       <c r="O41">
-        <v>1122.151763121045</v>
+        <v>1122.2</v>
       </c>
     </row>
     <row r="42">
@@ -2932,7 +2932,7 @@
         <v>14.5</v>
       </c>
       <c r="O42">
-        <v>1497.178338945776</v>
+        <v>1497.2</v>
       </c>
     </row>
     <row r="43">
@@ -2993,7 +2993,7 @@
         <v>13.3</v>
       </c>
       <c r="O43">
-        <v>1129.956526470114</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="44">
@@ -3054,7 +3054,7 @@
         <v>13.2</v>
       </c>
       <c r="O44">
-        <v>1158.644503385144</v>
+        <v>1158.6</v>
       </c>
     </row>
     <row r="45">
@@ -3115,7 +3115,7 @@
         <v>15.2</v>
       </c>
       <c r="O45">
-        <v>1584.736620596425</v>
+        <v>1584.7</v>
       </c>
     </row>
     <row r="46">
@@ -3176,7 +3176,7 @@
         <v>13.4</v>
       </c>
       <c r="O46">
-        <v>1062.396576454665</v>
+        <v>1062.4</v>
       </c>
     </row>
     <row r="47">
@@ -3237,7 +3237,7 @@
         <v>14</v>
       </c>
       <c r="O47">
-        <v>1467.542648246912</v>
+        <v>1467.5</v>
       </c>
     </row>
     <row r="48">
@@ -3298,7 +3298,7 @@
         <v>14</v>
       </c>
       <c r="O48">
-        <v>1231.504320207199</v>
+        <v>1231.5</v>
       </c>
     </row>
     <row r="49">
@@ -3359,7 +3359,7 @@
         <v>14.2</v>
       </c>
       <c r="O49">
-        <v>1404.193479584825</v>
+        <v>1404.2</v>
       </c>
     </row>
     <row r="50">
@@ -3420,7 +3420,7 @@
         <v>14.3</v>
       </c>
       <c r="O50">
-        <v>1445.454633898298</v>
+        <v>1445.5</v>
       </c>
     </row>
     <row r="51">
@@ -3481,7 +3481,7 @@
         <v>14.6</v>
       </c>
       <c r="O51">
-        <v>1540.222347090161</v>
+        <v>1540.2</v>
       </c>
     </row>
     <row r="52">
@@ -3542,7 +3542,7 @@
         <v>12.2</v>
       </c>
       <c r="O52">
-        <v>911.809568592594</v>
+        <v>911.8</v>
       </c>
     </row>
     <row r="53">
@@ -3603,7 +3603,7 @@
         <v>13.5</v>
       </c>
       <c r="O53">
-        <v>1059.227233065968</v>
+        <v>1059.2</v>
       </c>
     </row>
     <row r="54">
@@ -3664,7 +3664,7 @@
         <v>15.1</v>
       </c>
       <c r="O54">
-        <v>1516.199111666935</v>
+        <v>1516.2</v>
       </c>
     </row>
     <row r="55">
@@ -3725,7 +3725,7 @@
         <v>11.5</v>
       </c>
       <c r="O55">
-        <v>789.4036940307752</v>
+        <v>789.4</v>
       </c>
     </row>
     <row r="56">
@@ -3786,7 +3786,7 @@
         <v>13.6</v>
       </c>
       <c r="O56">
-        <v>1288.036232810996</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="57">
@@ -3847,7 +3847,7 @@
         <v>14.1</v>
       </c>
       <c r="O57">
-        <v>1249.160070920374</v>
+        <v>1249.2</v>
       </c>
     </row>
     <row r="58">
@@ -3908,7 +3908,7 @@
         <v>14.5</v>
       </c>
       <c r="O58">
-        <v>1398.100360633187</v>
+        <v>1398.1</v>
       </c>
     </row>
     <row r="59">
@@ -3969,7 +3969,7 @@
         <v>14.5</v>
       </c>
       <c r="O59">
-        <v>1464.152346174913</v>
+        <v>1464.2</v>
       </c>
     </row>
     <row r="60">
@@ -4030,7 +4030,7 @@
         <v>14.2</v>
       </c>
       <c r="O60">
-        <v>1266.941485339692</v>
+        <v>1266.9</v>
       </c>
     </row>
     <row r="61">
@@ -4091,7 +4091,7 @@
         <v>14.7</v>
       </c>
       <c r="O61">
-        <v>1482.192418389377</v>
+        <v>1482.2</v>
       </c>
     </row>
     <row r="62">
@@ -4152,7 +4152,7 @@
         <v>14.6</v>
       </c>
       <c r="O62">
-        <v>1596.027504593427</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="63">
@@ -4213,7 +4213,7 @@
         <v>12.5</v>
       </c>
       <c r="O63">
-        <v>989.9289351155337</v>
+        <v>989.9</v>
       </c>
     </row>
     <row r="64">
@@ -4274,7 +4274,7 @@
         <v>14.3</v>
       </c>
       <c r="O64">
-        <v>1338.383920276202</v>
+        <v>1338.4</v>
       </c>
     </row>
     <row r="65">
@@ -4335,7 +4335,7 @@
         <v>12.9</v>
       </c>
       <c r="O65">
-        <v>1071.724488641949</v>
+        <v>1071.7</v>
       </c>
     </row>
     <row r="66">
@@ -4396,7 +4396,7 @@
         <v>14.6</v>
       </c>
       <c r="O66">
-        <v>1484.417189586894</v>
+        <v>1484.4</v>
       </c>
     </row>
     <row r="67">
@@ -4457,7 +4457,7 @@
         <v>13.3</v>
       </c>
       <c r="O67">
-        <v>1139.218465211672</v>
+        <v>1139.2</v>
       </c>
     </row>
     <row r="68">
@@ -4518,7 +4518,7 @@
         <v>11.2</v>
       </c>
       <c r="O68">
-        <v>722.4825345215567</v>
+        <v>722.5</v>
       </c>
     </row>
     <row r="69">
@@ -4579,7 +4579,7 @@
         <v>14.2</v>
       </c>
       <c r="O69">
-        <v>1298.615022473184</v>
+        <v>1298.6</v>
       </c>
     </row>
     <row r="70">
@@ -4640,7 +4640,7 @@
         <v>13.2</v>
       </c>
       <c r="O70">
-        <v>976.180802064649</v>
+        <v>976.2000000000001</v>
       </c>
     </row>
     <row r="71">
@@ -4701,7 +4701,7 @@
         <v>14.1</v>
       </c>
       <c r="O71">
-        <v>1332.437408981732</v>
+        <v>1332.4</v>
       </c>
     </row>
     <row r="72">
@@ -4762,7 +4762,7 @@
         <v>14.2</v>
       </c>
       <c r="O72">
-        <v>1309.172868184348</v>
+        <v>1309.2</v>
       </c>
     </row>
     <row r="73">
@@ -4823,7 +4823,7 @@
         <v>14.7</v>
       </c>
       <c r="O73">
-        <v>1380.362404912244</v>
+        <v>1380.4</v>
       </c>
     </row>
     <row r="74">
@@ -4884,7 +4884,7 @@
         <v>13.3</v>
       </c>
       <c r="O74">
-        <v>1139.218465211672</v>
+        <v>1139.2</v>
       </c>
     </row>
     <row r="75">
@@ -4945,7 +4945,7 @@
         <v>12.8</v>
       </c>
       <c r="O75">
-        <v>986.5438690312908</v>
+        <v>986.5</v>
       </c>
     </row>
     <row r="76">
@@ -5006,7 +5006,7 @@
         <v>13</v>
       </c>
       <c r="O76">
-        <v>1017.614220375294</v>
+        <v>1017.6</v>
       </c>
     </row>
     <row r="77">
@@ -5067,7 +5067,7 @@
         <v>12.7</v>
       </c>
       <c r="O77">
-        <v>996.5247088917455</v>
+        <v>996.5</v>
       </c>
     </row>
     <row r="78">
@@ -5128,7 +5128,7 @@
         <v>14.1</v>
       </c>
       <c r="O78">
-        <v>1332.437408981732</v>
+        <v>1332.4</v>
       </c>
     </row>
     <row r="79">
@@ -5189,7 +5189,7 @@
         <v>13</v>
       </c>
       <c r="O79">
-        <v>1035.311858990516</v>
+        <v>1035.3</v>
       </c>
     </row>
     <row r="80">
@@ -5250,7 +5250,7 @@
         <v>14</v>
       </c>
       <c r="O80">
-        <v>1323.867144222739</v>
+        <v>1323.9</v>
       </c>
     </row>
     <row r="81">
@@ -5311,7 +5311,7 @@
         <v>13</v>
       </c>
       <c r="O81">
-        <v>1026.463039682905</v>
+        <v>1026.5</v>
       </c>
     </row>
     <row r="82">
@@ -5372,7 +5372,7 @@
         <v>13.6</v>
       </c>
       <c r="O82">
-        <v>1200.875886229801</v>
+        <v>1200.9</v>
       </c>
     </row>
     <row r="83">
@@ -5433,7 +5433,7 @@
         <v>12.8</v>
       </c>
       <c r="O83">
-        <v>943.6506573342782</v>
+        <v>943.7000000000001</v>
       </c>
     </row>
     <row r="84">
@@ -5494,7 +5494,7 @@
         <v>13</v>
       </c>
       <c r="O84">
-        <v>1123.800052066629</v>
+        <v>1123.8</v>
       </c>
     </row>
     <row r="85">
@@ -5555,7 +5555,7 @@
         <v>12.2</v>
       </c>
       <c r="O85">
-        <v>904.016324416589</v>
+        <v>904</v>
       </c>
     </row>
     <row r="86">
@@ -5616,7 +5616,7 @@
         <v>13.1</v>
       </c>
       <c r="O86">
-        <v>1132.170302093343</v>
+        <v>1132.2</v>
       </c>
     </row>
     <row r="87">
@@ -5677,7 +5677,7 @@
         <v>14</v>
       </c>
       <c r="O87">
-        <v>1313.604608221012</v>
+        <v>1313.6</v>
       </c>
     </row>
     <row r="88">
@@ -5738,7 +5738,7 @@
         <v>13</v>
       </c>
       <c r="O88">
-        <v>1008.765401067682</v>
+        <v>1008.8</v>
       </c>
     </row>
     <row r="89">
@@ -5799,7 +5799,7 @@
         <v>14.6</v>
       </c>
       <c r="O89">
-        <v>1372.806874580361</v>
+        <v>1372.8</v>
       </c>
     </row>
     <row r="90">
@@ -5860,7 +5860,7 @@
         <v>14.4</v>
       </c>
       <c r="O90">
-        <v>1444.026780037241</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="91">
@@ -5921,7 +5921,7 @@
         <v>13.3</v>
       </c>
       <c r="O91">
-        <v>1074.384894020764</v>
+        <v>1074.4</v>
       </c>
     </row>
     <row r="92">
@@ -5982,7 +5982,7 @@
         <v>14.7</v>
       </c>
       <c r="O92">
-        <v>1470.877972447473</v>
+        <v>1470.9</v>
       </c>
     </row>
     <row r="93">
@@ -6043,7 +6043,7 @@
         <v>11</v>
       </c>
       <c r="O93">
-        <v>747.5943317992511</v>
+        <v>747.6</v>
       </c>
     </row>
     <row r="94">
@@ -6104,7 +6104,7 @@
         <v>13.4</v>
       </c>
       <c r="O94">
-        <v>1090.601795298594</v>
+        <v>1090.6</v>
       </c>
     </row>
     <row r="95">
@@ -6165,7 +6165,7 @@
         <v>13.5</v>
       </c>
       <c r="O95">
-        <v>1164.195697604037</v>
+        <v>1164.2</v>
       </c>
     </row>
     <row r="96">
@@ -6226,7 +6226,7 @@
         <v>12.8</v>
       </c>
       <c r="O96">
-        <v>1012.279796049499</v>
+        <v>1012.3</v>
       </c>
     </row>
     <row r="97">
@@ -6287,7 +6287,7 @@
         <v>14.4</v>
       </c>
       <c r="O97">
-        <v>1324.595993718372</v>
+        <v>1324.6</v>
       </c>
     </row>
     <row r="98">
@@ -6348,7 +6348,7 @@
         <v>15</v>
       </c>
       <c r="O98">
-        <v>1578.650308428871</v>
+        <v>1578.7</v>
       </c>
     </row>
     <row r="99">
@@ -6409,7 +6409,7 @@
         <v>13.4</v>
       </c>
       <c r="O99">
-        <v>1203.422670674311</v>
+        <v>1203.4</v>
       </c>
     </row>
     <row r="100">
@@ -6470,7 +6470,7 @@
         <v>12.4</v>
       </c>
       <c r="O100">
-        <v>982.204282379132</v>
+        <v>982.2000000000001</v>
       </c>
     </row>
     <row r="101">
@@ -6531,7 +6531,7 @@
         <v>11.3</v>
       </c>
       <c r="O101">
-        <v>702.0124403895412</v>
+        <v>702</v>
       </c>
     </row>
     <row r="102">
@@ -6592,7 +6592,7 @@
         <v>13</v>
       </c>
       <c r="O102">
-        <v>1150.346509989462</v>
+        <v>1150.3</v>
       </c>
     </row>
     <row r="103">
@@ -6653,7 +6653,7 @@
         <v>11</v>
       </c>
       <c r="O103">
-        <v>658.8966992128993</v>
+        <v>658.9</v>
       </c>
     </row>
     <row r="104">
@@ -6714,7 +6714,7 @@
         <v>15</v>
       </c>
       <c r="O104">
-        <v>1496.183501272139</v>
+        <v>1496.2</v>
       </c>
     </row>
     <row r="105">
@@ -6775,7 +6775,7 @@
         <v>14</v>
       </c>
       <c r="O105">
-        <v>1405.967432236552</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="106">
@@ -6836,7 +6836,7 @@
         <v>12.5</v>
       </c>
       <c r="O106">
-        <v>1079.922474671491</v>
+        <v>1079.9</v>
       </c>
     </row>
     <row r="107">
@@ -6897,7 +6897,7 @@
         <v>14.7</v>
       </c>
       <c r="O107">
-        <v>1584.022431866509</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="108">
@@ -6958,7 +6958,7 @@
         <v>14.9</v>
       </c>
       <c r="O108">
-        <v>1534.422967051634</v>
+        <v>1534.4</v>
       </c>
     </row>
     <row r="109">
@@ -7019,7 +7019,7 @@
         <v>11.9</v>
       </c>
       <c r="O109">
-        <v>837.8590955209687</v>
+        <v>837.9</v>
       </c>
     </row>
     <row r="110">
@@ -7080,7 +7080,7 @@
         <v>11.7</v>
       </c>
       <c r="O110">
-        <v>759.7596257515019</v>
+        <v>759.8</v>
       </c>
     </row>
     <row r="111">
@@ -7141,7 +7141,7 @@
         <v>14.6</v>
       </c>
       <c r="O111">
-        <v>1462.095126585587</v>
+        <v>1462.1</v>
       </c>
     </row>
     <row r="112">
@@ -7202,7 +7202,7 @@
         <v>14.8</v>
       </c>
       <c r="O112">
-        <v>1571.240338556604</v>
+        <v>1571.2</v>
       </c>
     </row>
     <row r="113">
@@ -7263,7 +7263,7 @@
         <v>13.8</v>
       </c>
       <c r="O113">
-        <v>1236.455470229256</v>
+        <v>1236.5</v>
       </c>
     </row>
     <row r="114">
@@ -7324,7 +7324,7 @@
         <v>13.9</v>
       </c>
       <c r="O114">
-        <v>1183.624877370164</v>
+        <v>1183.6</v>
       </c>
     </row>
     <row r="115">
@@ -7385,7 +7385,7 @@
         <v>14.8</v>
       </c>
       <c r="O115">
-        <v>1479.489077910963</v>
+        <v>1479.5</v>
       </c>
     </row>
     <row r="116">
@@ -12802,7 +12802,7 @@
         <v>16.3</v>
       </c>
       <c r="O219">
-        <v>1905.874934035355</v>
+        <v>1905.9</v>
       </c>
     </row>
     <row r="220">
@@ -13539,7 +13539,7 @@
         <v>14.7</v>
       </c>
       <c r="O233">
-        <v>1595.336877808413</v>
+        <v>1595.3</v>
       </c>
     </row>
     <row r="234">
@@ -14068,7 +14068,7 @@
         <v>14.7</v>
       </c>
       <c r="O243">
-        <v>1482.192418389377</v>
+        <v>1482.2</v>
       </c>
     </row>
     <row r="244">
@@ -14805,7 +14805,7 @@
         <v>16.6</v>
       </c>
       <c r="O257">
-        <v>2120.958315476848</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="258">
@@ -16062,7 +16062,7 @@
         <v>15.8</v>
       </c>
       <c r="O281">
-        <v>1777.672297428887</v>
+        <v>1777.7</v>
       </c>
     </row>
     <row r="282">
@@ -17319,7 +17319,7 @@
         <v>14.8</v>
       </c>
       <c r="O305">
-        <v>1502.426893072373</v>
+        <v>1502.4</v>
       </c>
     </row>
     <row r="306">

</xml_diff>